<commit_message>
finito tutto, da ricontrollare
</commit_message>
<xml_diff>
--- a/Progetto_Gaeta/transitions rates matrix.xlsx
+++ b/Progetto_Gaeta/transitions rates matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorigr/Desktop/SimMod/Progetto_Gaeta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BB055F-0160-244E-8AC8-1D7E9FD1FB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C71445B-BEDE-0B43-B4EF-9200EB5D9456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{C89E0AF0-0222-D342-91A9-85DA70DAA525}"/>
   </bookViews>
@@ -45,162 +45,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
   <si>
     <t>Condizione di normalizzazione</t>
   </si>
   <si>
     <t>Termini noti</t>
-  </si>
-  <si>
-    <t>x1</t>
-  </si>
-  <si>
-    <t>x2</t>
-  </si>
-  <si>
-    <t>x3</t>
-  </si>
-  <si>
-    <t>x4</t>
-  </si>
-  <si>
-    <t>x5</t>
-  </si>
-  <si>
-    <t>x6</t>
-  </si>
-  <si>
-    <t>x7</t>
-  </si>
-  <si>
-    <t>x8</t>
-  </si>
-  <si>
-    <t>x9</t>
-  </si>
-  <si>
-    <t>x10</t>
-  </si>
-  <si>
-    <t>x11</t>
-  </si>
-  <si>
-    <t>x12</t>
-  </si>
-  <si>
-    <t>x13</t>
-  </si>
-  <si>
-    <t>x14</t>
-  </si>
-  <si>
-    <t>x15</t>
-  </si>
-  <si>
-    <t>x16</t>
-  </si>
-  <si>
-    <t>x17</t>
-  </si>
-  <si>
-    <t>x18</t>
-  </si>
-  <si>
-    <t>x19</t>
-  </si>
-  <si>
-    <t>x20</t>
-  </si>
-  <si>
-    <t>x21</t>
-  </si>
-  <si>
-    <t>x22</t>
-  </si>
-  <si>
-    <t>x23</t>
-  </si>
-  <si>
-    <t>x24</t>
-  </si>
-  <si>
-    <t>x25</t>
-  </si>
-  <si>
-    <t>x26</t>
-  </si>
-  <si>
-    <t>x27</t>
-  </si>
-  <si>
-    <t>x28</t>
-  </si>
-  <si>
-    <t>x29</t>
-  </si>
-  <si>
-    <t>x30</t>
-  </si>
-  <si>
-    <t>x31</t>
-  </si>
-  <si>
-    <t>x32</t>
-  </si>
-  <si>
-    <t>x33</t>
-  </si>
-  <si>
-    <t>x34</t>
-  </si>
-  <si>
-    <t>x35</t>
-  </si>
-  <si>
-    <t>x36</t>
-  </si>
-  <si>
-    <t>x37</t>
-  </si>
-  <si>
-    <t>x38</t>
-  </si>
-  <si>
-    <t>x39</t>
-  </si>
-  <si>
-    <t>x40</t>
-  </si>
-  <si>
-    <t>x41</t>
-  </si>
-  <si>
-    <t>x42</t>
-  </si>
-  <si>
-    <t>x43</t>
-  </si>
-  <si>
-    <t>x44</t>
-  </si>
-  <si>
-    <t>x45</t>
-  </si>
-  <si>
-    <t>x46</t>
-  </si>
-  <si>
-    <t>x47</t>
-  </si>
-  <si>
-    <t>x48</t>
-  </si>
-  <si>
-    <t>x49</t>
-  </si>
-  <si>
-    <t>x50</t>
   </si>
   <si>
     <t>Coda 0x000</t>
@@ -247,6 +97,171 @@
   <si>
     <t>Nella script matlab "Pi.m" sono state fatte le dovute traformazioni sulla matrice</t>
   </si>
+  <si>
+    <t>𝜋1</t>
+  </si>
+  <si>
+    <t>𝜋2</t>
+  </si>
+  <si>
+    <t>𝜋3</t>
+  </si>
+  <si>
+    <t>𝜋4</t>
+  </si>
+  <si>
+    <t>𝜋5</t>
+  </si>
+  <si>
+    <t>𝜋6</t>
+  </si>
+  <si>
+    <t>𝜋7</t>
+  </si>
+  <si>
+    <t>𝜋8</t>
+  </si>
+  <si>
+    <t>𝜋9</t>
+  </si>
+  <si>
+    <t>𝜋10</t>
+  </si>
+  <si>
+    <t>𝜋11</t>
+  </si>
+  <si>
+    <t>𝜋12</t>
+  </si>
+  <si>
+    <t>𝜋13</t>
+  </si>
+  <si>
+    <t>𝜋14</t>
+  </si>
+  <si>
+    <t>𝜋15</t>
+  </si>
+  <si>
+    <t>𝜋16</t>
+  </si>
+  <si>
+    <t>𝜋17</t>
+  </si>
+  <si>
+    <t>𝜋18</t>
+  </si>
+  <si>
+    <t>𝜋19</t>
+  </si>
+  <si>
+    <t>𝜋20</t>
+  </si>
+  <si>
+    <t>𝜋21</t>
+  </si>
+  <si>
+    <t>𝜋22</t>
+  </si>
+  <si>
+    <t>𝜋23</t>
+  </si>
+  <si>
+    <t>𝜋24</t>
+  </si>
+  <si>
+    <t>𝜋25</t>
+  </si>
+  <si>
+    <t>𝜋26</t>
+  </si>
+  <si>
+    <t>𝜋27</t>
+  </si>
+  <si>
+    <t>𝜋28</t>
+  </si>
+  <si>
+    <t>𝜋29</t>
+  </si>
+  <si>
+    <t>𝜋30</t>
+  </si>
+  <si>
+    <t>𝜋31</t>
+  </si>
+  <si>
+    <t>𝜋32</t>
+  </si>
+  <si>
+    <t>𝜋33</t>
+  </si>
+  <si>
+    <t>𝜋34</t>
+  </si>
+  <si>
+    <t>𝜋35</t>
+  </si>
+  <si>
+    <t>𝜋36</t>
+  </si>
+  <si>
+    <t>𝜋37</t>
+  </si>
+  <si>
+    <t>𝜋38</t>
+  </si>
+  <si>
+    <t>𝜋39</t>
+  </si>
+  <si>
+    <t>𝜋40</t>
+  </si>
+  <si>
+    <t>𝜋41</t>
+  </si>
+  <si>
+    <t>𝜋42</t>
+  </si>
+  <si>
+    <t>𝜋43</t>
+  </si>
+  <si>
+    <t>𝜋44</t>
+  </si>
+  <si>
+    <t>𝜋45</t>
+  </si>
+  <si>
+    <t>𝜋46</t>
+  </si>
+  <si>
+    <t>𝜋47</t>
+  </si>
+  <si>
+    <t>𝜋48</t>
+  </si>
+  <si>
+    <t>𝜋49</t>
+  </si>
+  <si>
+    <t>𝜋50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ro </t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>waiting time</t>
+  </si>
+  <si>
+    <t>per poi risolvere il sistema</t>
+  </si>
 </sst>
 </file>
 
@@ -289,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -397,21 +412,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -533,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -545,18 +545,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -874,10 +875,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AZ64"/>
+  <dimension ref="A1:AZ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="114" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q73" sqref="Q73"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="114" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9311,532 +9312,682 @@
     <row r="53" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B54" s="9" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="J54" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="K54" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L54" s="10" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="L54" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="M54" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N54" s="10" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="N54" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="O54" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="P54" s="10" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="P54" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="Q54" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="R54" s="10" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="R54" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="S54" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="T54" s="10" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="T54" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="U54" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="V54" s="10" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="V54" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="W54" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="X54" s="10" t="s">
-        <v>24</v>
+        <v>38</v>
+      </c>
+      <c r="X54" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="Y54" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z54" s="10" t="s">
-        <v>26</v>
+        <v>40</v>
+      </c>
+      <c r="Z54" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="AA54" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB54" s="10" t="s">
-        <v>28</v>
+        <v>42</v>
+      </c>
+      <c r="AB54" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="AC54" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD54" s="10" t="s">
-        <v>30</v>
+        <v>44</v>
+      </c>
+      <c r="AD54" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="AE54" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF54" s="10" t="s">
-        <v>32</v>
+        <v>46</v>
+      </c>
+      <c r="AF54" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="AG54" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH54" s="10" t="s">
-        <v>34</v>
+        <v>48</v>
+      </c>
+      <c r="AH54" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="AI54" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ54" s="10" t="s">
-        <v>36</v>
+        <v>50</v>
+      </c>
+      <c r="AJ54" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="AK54" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL54" s="10" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="AL54" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="AM54" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN54" s="10" t="s">
-        <v>40</v>
+        <v>54</v>
+      </c>
+      <c r="AN54" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="AO54" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP54" s="10" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="AP54" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="AQ54" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR54" s="10" t="s">
-        <v>44</v>
+        <v>58</v>
+      </c>
+      <c r="AR54" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="AS54" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="AT54" s="10" t="s">
-        <v>46</v>
+        <v>60</v>
+      </c>
+      <c r="AT54" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="AU54" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="AV54" s="10" t="s">
-        <v>48</v>
+        <v>62</v>
+      </c>
+      <c r="AV54" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="AW54" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX54" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AY54" s="11" t="s">
-        <v>51</v>
+        <v>64</v>
+      </c>
+      <c r="AX54" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AY54" s="10" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="12">
+      <c r="B55" s="11">
         <v>0.80785936519998502</v>
       </c>
-      <c r="C55" s="13">
+      <c r="C55" s="12">
         <v>4.8446743271680004E-3</v>
       </c>
-      <c r="D55" s="13">
+      <c r="D55" s="12">
         <v>2.4856383640867001E-2</v>
       </c>
-      <c r="E55" s="13">
+      <c r="E55" s="12">
         <v>1.668489239463E-3</v>
       </c>
-      <c r="F55" s="15">
+      <c r="F55" s="14">
         <v>9.9291777187E-5</v>
       </c>
-      <c r="G55" s="15">
+      <c r="G55" s="14">
         <v>6.9251984711000001E-5</v>
       </c>
-      <c r="H55" s="13">
+      <c r="H55" s="12">
         <v>7.4889074547499998E-4</v>
       </c>
-      <c r="I55" s="15">
+      <c r="I55" s="14">
         <v>1.460693928E-6</v>
       </c>
-      <c r="J55" s="15">
+      <c r="J55" s="14">
         <v>7.3034696399999996E-6</v>
       </c>
-      <c r="K55" s="15">
+      <c r="K55" s="14">
         <v>2.2990712078000001E-5</v>
       </c>
-      <c r="L55" s="15">
+      <c r="L55" s="14">
         <v>1.9380105899999999E-5</v>
       </c>
-      <c r="M55" s="13">
+      <c r="M55" s="12">
         <v>4.2823263020742998E-2</v>
       </c>
-      <c r="N55" s="13">
+      <c r="N55" s="12">
         <v>2.8718603148463001E-2</v>
       </c>
-      <c r="O55" s="15">
+      <c r="O55" s="14">
         <v>3.8760211999999999E-8</v>
       </c>
-      <c r="P55" s="13">
+      <c r="P55" s="12">
         <v>1.6912052943400001E-4</v>
       </c>
-      <c r="Q55" s="13">
+      <c r="Q55" s="12">
         <v>1.3583794896500001E-4</v>
       </c>
-      <c r="R55" s="15">
+      <c r="R55" s="14">
         <v>2.1796365999999999E-7</v>
       </c>
-      <c r="S55" s="15">
+      <c r="S55" s="14">
         <v>3.3496074000000001E-7</v>
       </c>
-      <c r="T55" s="15">
+      <c r="T55" s="14">
         <v>2.7201977299999999E-7</v>
       </c>
-      <c r="U55" s="13">
+      <c r="U55" s="12">
         <v>9.5543330798800001E-4</v>
       </c>
-      <c r="V55" s="13">
+      <c r="V55" s="12">
         <v>2.6442057880206999E-2</v>
       </c>
-      <c r="W55" s="15">
+      <c r="W55" s="14">
         <v>4.470795527E-6</v>
       </c>
-      <c r="X55" s="15">
+      <c r="X55" s="14">
         <v>7.3956185281999997E-5</v>
       </c>
-      <c r="Y55" s="13">
+      <c r="Y55" s="12">
         <v>2.1779456407136001E-2</v>
       </c>
-      <c r="Z55" s="15">
+      <c r="Z55" s="14">
         <v>1.2885703E-8</v>
       </c>
-      <c r="AA55" s="15">
+      <c r="AA55" s="14">
         <v>7.2763723761000006E-5</v>
       </c>
-      <c r="AB55" s="15">
+      <c r="AB55" s="14">
         <v>5.4866578469999996E-6</v>
       </c>
-      <c r="AC55" s="15">
+      <c r="AC55" s="14">
         <v>2.057800112E-6</v>
       </c>
-      <c r="AD55" s="15">
+      <c r="AD55" s="14">
         <v>5.2960550178000002E-5</v>
       </c>
-      <c r="AE55" s="15">
+      <c r="AE55" s="14">
         <v>7.9417042837999995E-5</v>
       </c>
-      <c r="AF55" s="13">
+      <c r="AF55" s="12">
         <v>1.8514319362278001E-2</v>
       </c>
-      <c r="AG55" s="15">
+      <c r="AG55" s="14">
         <v>1.4033915899999999E-7</v>
       </c>
-      <c r="AH55" s="15">
+      <c r="AH55" s="14">
         <v>1.9970856714000001E-5</v>
       </c>
-      <c r="AI55" s="15">
+      <c r="AI55" s="14">
         <v>8.5418556029999995E-6</v>
       </c>
-      <c r="AJ55" s="13">
+      <c r="AJ55" s="12">
         <v>1.3171139690140001E-3</v>
       </c>
-      <c r="AK55" s="13">
+      <c r="AK55" s="12">
         <v>1.7234480255057999E-2</v>
       </c>
-      <c r="AL55" s="15">
+      <c r="AL55" s="14">
         <v>8.7769694900000003E-7</v>
       </c>
-      <c r="AM55" s="15">
+      <c r="AM55" s="14">
         <v>3.471104209E-6</v>
       </c>
-      <c r="AN55" s="15">
+      <c r="AN55" s="14">
         <v>2.6263673959999999E-6</v>
       </c>
-      <c r="AO55" s="15">
+      <c r="AO55" s="14">
         <v>9.0879414999999999E-8</v>
       </c>
-      <c r="AP55" s="15">
+      <c r="AP55" s="14">
         <v>1.8629956403E-5</v>
       </c>
-      <c r="AQ55" s="15">
+      <c r="AQ55" s="14">
         <v>4.0543181349999997E-6</v>
       </c>
-      <c r="AR55" s="15">
+      <c r="AR55" s="14">
         <v>2.2694256710000001E-5</v>
       </c>
-      <c r="AS55" s="13">
+      <c r="AS55" s="12">
         <v>1.337318688606E-3</v>
       </c>
-      <c r="AT55" s="15">
+      <c r="AT55" s="14">
         <v>2.1862774640000001E-6</v>
       </c>
-      <c r="AU55" s="15">
+      <c r="AU55" s="14">
         <v>1.18812485E-7</v>
       </c>
-      <c r="AV55" s="15">
+      <c r="AV55" s="14">
         <v>1.8941841000000001E-8</v>
       </c>
-      <c r="AW55" s="15">
+      <c r="AW55" s="14">
         <v>9.3103862E-8</v>
       </c>
-      <c r="AX55" s="15">
+      <c r="AX55" s="14">
         <v>5.1238630000000003E-9</v>
       </c>
-      <c r="AY55" s="16">
+      <c r="AY55" s="15">
         <v>4.3498630000000002E-9</v>
       </c>
     </row>
     <row r="58" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="B58" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" s="18"/>
-      <c r="E58" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F58" s="18"/>
-      <c r="H58" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="I58" s="18"/>
-      <c r="K58" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="L58" s="18"/>
-      <c r="N58" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="O58" s="18"/>
+      <c r="B58" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="17"/>
+      <c r="E58" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F58" s="17"/>
+      <c r="H58" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I58" s="17"/>
+      <c r="K58" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="L58" s="17"/>
+      <c r="N58" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O58" s="17"/>
       <c r="Q58" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="B59" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C59" s="20">
+      <c r="B59" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="19">
         <f>SUM(I55,J55,K55,O55,R55,S55,T55,X55,Y55,Z55,AC55,AD55,AE55,AF55,AG55,AH55,AI55,AL55,AN55,AO55,AP55,AQ55,AR55,AS55,AT55,AU55,AV55,AW55,AX55,AY55)</f>
         <v>4.1952170638026004E-2</v>
       </c>
-      <c r="E59" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F59" s="20">
+      <c r="E59" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="19">
         <f>SUM(B55,D55,E55,G55,H55,J55,K55,M55,N55,U55,V55,X55,Y55,AA55,AB55,AE55,AF55,AH55,AI55,AJ55,AK55,AL55,AM55,AR55,AS55,AT55,AU55,AW55,AX55,AY55)</f>
         <v>0.99464430807916171</v>
       </c>
-      <c r="H59" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="I59" s="20">
+      <c r="H59" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I59" s="19">
         <f>SUM(B55,F55,C55,D55,H55,I55,J55,L55,M55,N55,O55,P55,Q55,R55,S55,T55,U55,V55,X55,Y55,AC55,AD55,AE55,AF55,AJ55,AK55,AN55,AQ55,AR55,AS55)</f>
         <v>0.99810238470307799</v>
       </c>
-      <c r="K59" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="L59" s="20">
+      <c r="K59" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="L59" s="19">
         <f>SUM(B55,C55,E55,L55,M55,N55,O55,P55,Q55,S55,T55,W55,Z55,AA55,AB55,AJ55,AK55,AM55,AN55,AO55,AP55,AQ55,AR55,AS55,AT55,AU55,AV55,AW55,AX55,AY55)</f>
         <v>0.90626501972800777</v>
       </c>
-      <c r="N59" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="O59" s="20">
+      <c r="N59" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="O59" s="19">
         <f>SUM(O55,B55,C55,D55,E55,F55,G55,H55,I55,J55,K55,L55,P55,R55,W55,Z55,AG55,AL55,AM55,AV55,AY55)</f>
         <v>0.84037585526295877</v>
       </c>
+      <c r="Q59" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="60" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="B60" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C60" s="20">
+      <c r="B60" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="19">
         <f>SUM(G55,H55,L55,P55,Q55,U55,V55,W55,AA55,AB55,AJ55,AK55,AM55,F55)</f>
         <v>4.7277050785282999E-2</v>
       </c>
-      <c r="E60" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F60" s="20">
+      <c r="E60" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60" s="19">
         <f xml:space="preserve"> SUM(C55,F55,I55,P55,Q55,W55,AC55,AD55,AG55,AN55,AO55,AP55,AQ55,AV55)</f>
         <v>5.3354352248480017E-3</v>
       </c>
-      <c r="H60" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I60" s="20">
+      <c r="H60" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I60" s="19">
         <f>SUM(E55,G55,K55,W55,Z55,AA55,AB55,AG55,AH55,AI55,AO55,AP55,AT55,AU55)</f>
         <v>1.8931449763330002E-3</v>
       </c>
-      <c r="K60" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="L60" s="20">
+      <c r="K60" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="L60" s="19">
         <f>SUM(D55,F55,G55,R55,U55,V55,AC55,AD55,AE55,AF55,AG55,AH55,AI55,AL55)</f>
         <v>7.1100922058450991E-2</v>
       </c>
-      <c r="N60" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="O60" s="20">
+      <c r="N60" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O60" s="19">
         <f>SUM(M55,N55,O55,Q55,S55,T55,U55,V55,X55,Y55,AA55,AB55,AC55,AD55,AH55,AI55,AO55,AP55,AW55,AX55)</f>
         <v>0.12110985414726699</v>
       </c>
     </row>
     <row r="61" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="B61" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C61" s="20">
+      <c r="B61" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="19">
         <f>SUM(C55,D55,E55,L55,N55)</f>
         <v>6.0107530461861007E-2</v>
       </c>
-      <c r="E61" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F61" s="20">
+      <c r="E61" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="19">
         <f>SUM(L55,R55,S55,T55,Z55)</f>
         <v>2.0217935775999999E-5</v>
       </c>
-      <c r="H61" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="I61" s="20">
+      <c r="H61" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I61" s="19">
         <f>SUM(AL55,AM55,AV55,AW55,AX55)</f>
         <v>4.4659707240000002E-6</v>
       </c>
-      <c r="K61" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="L61" s="20">
+      <c r="K61" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="L61" s="19">
         <f>SUM(H55,I55,K55,X55,Y55)</f>
         <v>2.2626754743899E-2</v>
       </c>
-      <c r="N61" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="O61" s="20">
+      <c r="N61" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="O61" s="19">
         <f>SUM(AE55,AF55,AJ55,AK55,AN55,AQ55,AT55,AU55)</f>
         <v>3.7154316404668E-2</v>
       </c>
     </row>
     <row r="62" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="B62" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C62" s="20">
+      <c r="B62" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="19">
         <f>B55</f>
         <v>0.80785936519998502</v>
       </c>
-      <c r="E62" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F62" s="20">
+      <c r="E62" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" s="19">
         <f>O55</f>
         <v>3.8760211999999999E-8</v>
       </c>
-      <c r="H62" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="I62" s="20">
+      <c r="H62" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I62" s="19">
         <f>AY55</f>
         <v>4.3498630000000002E-9</v>
       </c>
-      <c r="K62" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="L62" s="20">
+      <c r="K62" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="L62" s="19">
         <f>J55</f>
         <v>7.3034696399999996E-6</v>
       </c>
-      <c r="N62" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="O62" s="20">
+      <c r="N62" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="O62" s="19">
         <f>SUM(AR55,AS55)</f>
         <v>1.360012945316E-3</v>
       </c>
     </row>
     <row r="63" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="B63" s="19"/>
-      <c r="C63" s="20"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="20"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="20"/>
-      <c r="K63" s="19"/>
-      <c r="L63" s="20"/>
-      <c r="N63" s="19"/>
-      <c r="O63" s="20"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="19"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="19"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="19"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="19"/>
+      <c r="N63" s="18"/>
+      <c r="O63" s="19"/>
     </row>
     <row r="64" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="B64" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C64" s="22">
+      <c r="B64" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="23">
         <f>C60+C61*2+C62*3</f>
         <v>2.59107020730896</v>
       </c>
-      <c r="D64" s="14"/>
-      <c r="E64" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="F64" s="22">
+      <c r="D64" s="13"/>
+      <c r="E64" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" s="23">
         <f>F60+F61*2+F62*3</f>
         <v>5.3759873770360019E-3</v>
       </c>
-      <c r="G64" s="14"/>
-      <c r="H64" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="I64" s="22">
+      <c r="G64" s="13"/>
+      <c r="H64" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I64" s="23">
         <f>I60+I61*2+I62*3</f>
         <v>1.9020899673700003E-3</v>
       </c>
-      <c r="J64" s="14"/>
-      <c r="K64" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="L64" s="22">
+      <c r="J64" s="13"/>
+      <c r="K64" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="L64" s="23">
         <f>L60+L61*2+L62*3</f>
         <v>0.11637634195516899</v>
       </c>
-      <c r="M64" s="14"/>
-      <c r="N64" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="O64" s="22">
+      <c r="M64" s="13"/>
+      <c r="N64" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O64" s="23">
         <f>O60+O61*2+O62*3</f>
         <v>0.19949852579255101</v>
+      </c>
+    </row>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B65" s="18"/>
+      <c r="C65" s="19"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="19"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="19"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="19"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="19"/>
+    </row>
+    <row r="66" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B66" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" s="19">
+        <f>1-C59</f>
+        <v>0.95804782936197397</v>
+      </c>
+      <c r="E66" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F66" s="19">
+        <f>1-F59</f>
+        <v>5.3556919208382903E-3</v>
+      </c>
+      <c r="H66" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I66" s="19">
+        <f>1-I59</f>
+        <v>1.8976152969220061E-3</v>
+      </c>
+      <c r="K66" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="L66" s="19">
+        <f>1-L59</f>
+        <v>9.373498027199223E-2</v>
+      </c>
+      <c r="N66" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="O66" s="19">
+        <f>1-O59</f>
+        <v>0.15962414473704123</v>
+      </c>
+    </row>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B67" s="18"/>
+      <c r="C67" s="19"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="19"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="19"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="19"/>
+      <c r="N67" s="18"/>
+      <c r="O67" s="19"/>
+    </row>
+    <row r="68" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B68" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="19">
+        <f>C66/2500</f>
+        <v>3.8321913174478958E-4</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F68" s="19">
+        <f>F66/5</f>
+        <v>1.0711383841676581E-3</v>
+      </c>
+      <c r="H68" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I68" s="19">
+        <f>I66/4</f>
+        <v>4.7440382423050154E-4</v>
+      </c>
+      <c r="K68" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="L68" s="19">
+        <f>L66/50</f>
+        <v>1.8746996054398446E-3</v>
+      </c>
+      <c r="N68" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="O68" s="19">
+        <f>O66/200</f>
+        <v>7.981207236852062E-4</v>
+      </c>
+    </row>
+    <row r="69" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B69" s="18"/>
+      <c r="C69" s="19"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="19"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="19"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="19"/>
+      <c r="N69" s="18"/>
+      <c r="O69" s="19"/>
+    </row>
+    <row r="70" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B70" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" s="21">
+        <f>C64/C68</f>
+        <v>6761.3279000760358</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F70" s="21">
+        <f xml:space="preserve"> F64/F68</f>
+        <v>5.0189475575683735</v>
+      </c>
+      <c r="H70" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="I70" s="21">
+        <f>I64/I68</f>
+        <v>4.0094321972535791</v>
+      </c>
+      <c r="K70" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="L70" s="21">
+        <f>L64/L68</f>
+        <v>62.077327811601378</v>
+      </c>
+      <c r="N70" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="O70" s="21">
+        <f>O64/O68</f>
+        <v>249.96033791905018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>